<commit_message>
added DriverScript and AppTest on 22nd March
</commit_message>
<xml_diff>
--- a/FileInput/Controller.xlsx
+++ b/FileInput/Controller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Automation Testing\Qedge\Project\sample_project\HybridFramework\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FDB795-3A8D-49B3-B68B-712C7EE412BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C43CFE7-802F-4852-AB64-0438B84F46F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11316" yWindow="948" windowWidth="10884" windowHeight="11856" activeTab="1" xr2:uid="{CD0C539F-FCD3-42BC-A1A6-244B63839D95}"/>
+    <workbookView xWindow="9732" yWindow="432" windowWidth="10884" windowHeight="11856" xr2:uid="{CD0C539F-FCD3-42BC-A1A6-244B63839D95}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -574,9 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F980FD02-E924-4C03-B5C6-DF0B84272D2D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -657,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F3D147-4E56-4439-A4A4-DB0B9E5AD231}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added StockItems module code on march 22
</commit_message>
<xml_diff>
--- a/FileInput/Controller.xlsx
+++ b/FileInput/Controller.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Automation Testing\Qedge\Project\sample_project\HybridFramework\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C43CFE7-802F-4852-AB64-0438B84F46F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E48CF9-786F-424A-ADB2-795FDD870D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9732" yWindow="432" windowWidth="10884" windowHeight="11856" xr2:uid="{CD0C539F-FCD3-42BC-A1A6-244B63839D95}"/>
+    <workbookView xWindow="11916" yWindow="144" windowWidth="10884" windowHeight="11856" xr2:uid="{CD0C539F-FCD3-42BC-A1A6-244B63839D95}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="92">
   <si>
     <t>TCID</t>
   </si>
@@ -182,13 +182,145 @@
   </si>
   <si>
     <t>Dashboard « Stock Accounting</t>
+  </si>
+  <si>
+    <t>ObjectType</t>
+  </si>
+  <si>
+    <t>Launch Url</t>
+  </si>
+  <si>
+    <t>openUrl</t>
+  </si>
+  <si>
+    <t>Enter username</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>validate page title</t>
+  </si>
+  <si>
+    <t>Wait for stock item link</t>
+  </si>
+  <si>
+    <t>//a[text()='Stock Items ']</t>
+  </si>
+  <si>
+    <t>Click Stock items link</t>
+  </si>
+  <si>
+    <t>Wait for Add Icon</t>
+  </si>
+  <si>
+    <t>(//span[@data-caption='Add'])[1]</t>
+  </si>
+  <si>
+    <t>Click Add icon</t>
+  </si>
+  <si>
+    <t>Wait for Category Listbox</t>
+  </si>
+  <si>
+    <t>x_Category</t>
+  </si>
+  <si>
+    <t>Select item in Category</t>
+  </si>
+  <si>
+    <t>dropDownAction</t>
+  </si>
+  <si>
+    <t>//select[@id='x_Category']</t>
+  </si>
+  <si>
+    <t>Seelct item in Supplier Number</t>
+  </si>
+  <si>
+    <t>x_Supplier_Number</t>
+  </si>
+  <si>
+    <t>Capture Stock number</t>
+  </si>
+  <si>
+    <t>captureStock</t>
+  </si>
+  <si>
+    <t>x_Stock_Number</t>
+  </si>
+  <si>
+    <t>Enter Stcok name</t>
+  </si>
+  <si>
+    <t>x_Stock_Name</t>
+  </si>
+  <si>
+    <t>Puzzels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select item in Unit Of Measurement </t>
+  </si>
+  <si>
+    <t>x_Unit_Of_Measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Purchasing Price </t>
+  </si>
+  <si>
+    <t>x_Purchasing_Price</t>
+  </si>
+  <si>
+    <t>Enter Selling Price</t>
+  </si>
+  <si>
+    <t>x_Selling_Price</t>
+  </si>
+  <si>
+    <t>Enter notes</t>
+  </si>
+  <si>
+    <t>x_Notes</t>
+  </si>
+  <si>
+    <t>Selling Puzzles</t>
+  </si>
+  <si>
+    <t>Click add button</t>
+  </si>
+  <si>
+    <t>btnAction</t>
+  </si>
+  <si>
+    <t>Wait for Confirm ok button</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='OK!']</t>
+  </si>
+  <si>
+    <t>Click Confirm ok button</t>
+  </si>
+  <si>
+    <t>Wait for alert ok</t>
+  </si>
+  <si>
+    <t>(//button[starts-with(text(),'OK')])[6]</t>
+  </si>
+  <si>
+    <t>Click Alert ok</t>
+  </si>
+  <si>
+    <t>Verify Stock Number</t>
+  </si>
+  <si>
+    <t>stockTable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +337,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,13 +399,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,7 +727,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F980FD02-E924-4C03-B5C6-DF0B84272D2D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -605,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -617,7 +772,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -875,36 +1030,647 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B50D6E-4E31-4DF3-BDFE-EF3B94316A4F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="5">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="6">
+        <v>10</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="6">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="6">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="5">
+        <v>300000</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="5">
+        <v>500000</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="5">
+        <v>10</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="5">
+        <v>10</v>
+      </c>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67806BB3-F6C2-4439-A2D7-0B121B1A3D38}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA02A28D-9C1D-48ED-A40B-E52CDD391D49}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G10:G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>